<commit_message>
Added CandidatesView and PasswordReset
</commit_message>
<xml_diff>
--- a/public/candidates.xlsx
+++ b/public/candidates.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>CANDIDATE_ID</t>
   </si>
@@ -35,6 +35,9 @@
     <t>EMAIL_ADDRESS</t>
   </si>
   <si>
+    <t>ORGANISATION</t>
+  </si>
+  <si>
     <t>WORK_LOCATION</t>
   </si>
   <si>
@@ -65,19 +68,28 @@
     <t>RECRUITER</t>
   </si>
   <si>
-    <t>00_CV sent to client</t>
-  </si>
-  <si>
-    <t>Karthik C M</t>
-  </si>
-  <si>
-    <t>karthikcm5329@gmail.com</t>
-  </si>
-  <si>
-    <t>Agartala</t>
-  </si>
-  <si>
-    <t>2022-10-14 01:38:23</t>
+    <t>01_Reject-No Show</t>
+  </si>
+  <si>
+    <t>Vinod Uttam Chavan</t>
+  </si>
+  <si>
+    <t>["8208909261",""]</t>
+  </si>
+  <si>
+    <t>vinodchavan3371@gmail.com</t>
+  </si>
+  <si>
+    <t>Facile info serv Pvt</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>2022-11-18 11:37:36</t>
+  </si>
+  <si>
+    <t>2022-11-19 12:30:00</t>
   </si>
 </sst>
 </file>
@@ -413,7 +425,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,8 +482,11 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1</v>
       </c>
@@ -479,39 +494,44 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2"/>
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2">
-        <v>3.6</v>
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
       </c>
       <c r="I2">
-        <v>3.9</v>
+        <v>4.4</v>
       </c>
       <c r="J2">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
       <c r="K2">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2"/>
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
       <c r="O2"/>
-      <c r="P2">
+      <c r="P2"/>
+      <c r="Q2">
         <v>1</v>
       </c>
     </row>

</xml_diff>